<commit_message>
Champs collection User en anglais
</commit_message>
<xml_diff>
--- a/project_ws/WS_List.xlsx
+++ b/project_ws/WS_List.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="22995" windowHeight="10035"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="22995" windowHeight="10035" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="WS" sheetId="1" r:id="rId1"/>
+    <sheet name="User" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>WS list</t>
   </si>
@@ -87,6 +87,36 @@
   </si>
   <si>
     <t>{pseudo_exists : boolean value}</t>
+  </si>
+  <si>
+    <t>User collection fields</t>
+  </si>
+  <si>
+    <t>Field name</t>
+  </si>
+  <si>
+    <t>_id</t>
+  </si>
+  <si>
+    <t>userLogin</t>
+  </si>
+  <si>
+    <t>userPwd</t>
+  </si>
+  <si>
+    <t>userLastName</t>
+  </si>
+  <si>
+    <t>userName</t>
+  </si>
+  <si>
+    <t>userEmail</t>
+  </si>
+  <si>
+    <t>userCountry</t>
+  </si>
+  <si>
+    <t>userSubmittedChoices</t>
   </si>
 </sst>
 </file>
@@ -139,7 +169,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -364,11 +394,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -419,6 +486,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -733,8 +803,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -883,13 +953,71 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="21.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" s="18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" s="19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6" s="19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B7" s="19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B8" s="19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9" s="19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B10" s="19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="20" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>